<commit_message>
Minor correction to the docs.
</commit_message>
<xml_diff>
--- a/doc/Fixed-data-types.xlsx
+++ b/doc/Fixed-data-types.xlsx
@@ -53,6 +53,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -70,21 +71,24 @@
       <family val="0"/>
     </font>
     <font>
-      <u val="single"/>
       <sz val="10"/>
       <name val="Lucida Sans"/>
       <family val="2"/>
-    </font>
-    <font>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u val="single"/>
       <sz val="10"/>
       <name val="Lucida Sans"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -128,9 +132,11 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="90" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="3">
@@ -154,8 +160,8 @@
     <cellStyle name="Currency" xfId="17" builtinId="4"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
-    <cellStyle name="Result2" xfId="20"/>
-    <cellStyle name="Heading1" xfId="21"/>
+    <cellStyle name="Heading 1" xfId="20"/>
+    <cellStyle name="Result2" xfId="21"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -168,7 +174,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
+      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3:E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -214,8 +220,8 @@
         <v>8192</v>
       </c>
       <c r="E3" s="1" t="n">
-        <f aca="false">C3*16</f>
-        <v>4194304</v>
+        <f aca="false">C3*16*2</f>
+        <v>8388608</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -234,8 +240,8 @@
         <v>4</v>
       </c>
       <c r="E4" s="1" t="n">
-        <f aca="false">C4*16</f>
-        <v>131072</v>
+        <f aca="false">C4*16*2</f>
+        <v>262144</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -254,8 +260,8 @@
         <v>16</v>
       </c>
       <c r="E5" s="1" t="n">
-        <f aca="false">C5*16</f>
-        <v>32768</v>
+        <f aca="false">C5*16*2</f>
+        <v>65536</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -274,8 +280,8 @@
         <v>32</v>
       </c>
       <c r="E6" s="1" t="n">
-        <f aca="false">C6*16</f>
-        <v>16384</v>
+        <f aca="false">C6*16*2</f>
+        <v>32768</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -294,8 +300,8 @@
         <v>64</v>
       </c>
       <c r="E7" s="1" t="n">
-        <f aca="false">C7*16</f>
-        <v>8192</v>
+        <f aca="false">C7*16*2</f>
+        <v>16384</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -314,8 +320,8 @@
         <v>128</v>
       </c>
       <c r="E8" s="1" t="n">
-        <f aca="false">C8*16</f>
-        <v>4096</v>
+        <f aca="false">C8*16*2</f>
+        <v>8192</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -334,8 +340,8 @@
         <v>8192</v>
       </c>
       <c r="E9" s="1" t="n">
-        <f aca="false">C9*16</f>
-        <v>64</v>
+        <f aca="false">C9*16*2</f>
+        <v>128</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -354,8 +360,8 @@
         <v>512</v>
       </c>
       <c r="E10" s="1" t="n">
-        <f aca="false">C10*16</f>
-        <v>67108864</v>
+        <f aca="false">C10*16*2</f>
+        <v>134217728</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -375,14 +381,14 @@
         <v>1024</v>
       </c>
       <c r="E11" s="1" t="n">
-        <f aca="false">C11*16</f>
-        <v>8192</v>
+        <f aca="false">C11*16*2</f>
+        <v>16384</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>

</xml_diff>